<commit_message>
Updated example 1 and 2 for new SimulatorToFMU and JModelica 2.4. Added a variable to add the paths for SimulatorToFMU and fmi-for-power-systems in the first box, to adapt easily to individual computers
</commit_message>
<xml_diff>
--- a/examples/001_cosimulation/pandapower/pandapower.xlsx
+++ b/examples/001_cosimulation/pandapower/pandapower.xlsx
@@ -2,9 +2,8 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -12,6 +11,53 @@
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="14">
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>causality</t>
+  </si>
+  <si>
+    <t>start</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>unit</t>
+  </si>
+  <si>
+    <t>KW_7</t>
+  </si>
+  <si>
+    <t>_</t>
+  </si>
+  <si>
+    <t>input</t>
+  </si>
+  <si>
+    <t>Real</t>
+  </si>
+  <si>
+    <t>KVAR_7</t>
+  </si>
+  <si>
+    <t>Vpu_7</t>
+  </si>
+  <si>
+    <t>output</t>
+  </si>
+  <si>
+    <t>Vpu_12</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -366,156 +412,104 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>causality</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>start</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>unit</t>
-        </is>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>KW_7</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>_</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Real</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>_</t>
-        </is>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>KVAR_7</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>_</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>input</t>
-        </is>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Real</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>_</t>
-        </is>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Vpu_7</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>_</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>output</t>
-        </is>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
       </c>
       <c r="D4" t="n">
         <v>1</v>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Real</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>_</t>
-        </is>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Vpu_12</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>_</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>output</t>
-        </is>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
       </c>
       <c r="D5" t="n">
         <v>1</v>
       </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Real</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>_</t>
-        </is>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>